<commit_message>
Updated team report + test result files
</commit_message>
<xml_diff>
--- a/TeamAaronAshishJuliaReport.xlsx
+++ b/TeamAaronAshishJuliaReport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6300" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="271">
   <si>
     <t>Sprint</t>
   </si>
@@ -689,12 +689,6 @@
     <t>Complete</t>
   </si>
   <si>
-    <t>US_42.txt</t>
-  </si>
-  <si>
-    <t>US_38.txt</t>
-  </si>
-  <si>
     <t>us_42</t>
   </si>
   <si>
@@ -708,18 +702,6 @@
   </si>
   <si>
     <t>test_us38</t>
-  </si>
-  <si>
-    <t>US_04.txt</t>
-  </si>
-  <si>
-    <t>US_05.txt</t>
-  </si>
-  <si>
-    <t>US_22.txt</t>
-  </si>
-  <si>
-    <t>US_01.txt</t>
   </si>
   <si>
     <t>us_04</t>
@@ -805,6 +787,66 @@
   <si>
     <t>243-253</t>
   </si>
+  <si>
+    <t>us_06</t>
+  </si>
+  <si>
+    <t>us_07</t>
+  </si>
+  <si>
+    <t>us_08</t>
+  </si>
+  <si>
+    <t>us_16</t>
+  </si>
+  <si>
+    <t>test_us06</t>
+  </si>
+  <si>
+    <t>test_us07</t>
+  </si>
+  <si>
+    <t>test_us36</t>
+  </si>
+  <si>
+    <t>test_us35</t>
+  </si>
+  <si>
+    <t>test_us08</t>
+  </si>
+  <si>
+    <t>test_us16</t>
+  </si>
+  <si>
+    <t>331-345</t>
+  </si>
+  <si>
+    <t>313-328</t>
+  </si>
+  <si>
+    <t>294-310</t>
+  </si>
+  <si>
+    <t>275-291</t>
+  </si>
+  <si>
+    <t>103-107</t>
+  </si>
+  <si>
+    <t>111-117</t>
+  </si>
+  <si>
+    <t>66-72</t>
+  </si>
+  <si>
+    <t>77-83</t>
+  </si>
+  <si>
+    <t>87-91</t>
+  </si>
+  <si>
+    <t>95-99</t>
+  </si>
 </sst>
 </file>
 
@@ -814,7 +856,7 @@
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -909,6 +951,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -949,7 +1004,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1027,7 +1082,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1085,6 +1143,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1186,10 +1245,10 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1258,6 +1317,9 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -1398,6 +1460,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -31706,8 +31769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.41015625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -31992,8 +32055,8 @@
       <c r="D8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>13</v>
+      <c r="E8" s="24" t="s">
+        <v>217</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -32029,8 +32092,8 @@
       <c r="D9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>13</v>
+      <c r="E9" s="24" t="s">
+        <v>217</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -32066,8 +32129,8 @@
       <c r="D10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>13</v>
+      <c r="E10" s="24" t="s">
+        <v>217</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -32103,8 +32166,8 @@
       <c r="D11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>13</v>
+      <c r="E11" s="24" t="s">
+        <v>217</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -32140,8 +32203,8 @@
       <c r="D12" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>13</v>
+      <c r="E12" s="24" t="s">
+        <v>217</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -32177,8 +32240,8 @@
       <c r="D13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>13</v>
+      <c r="E13" s="24" t="s">
+        <v>217</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -40662,7 +40725,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.41015625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -40733,49 +40796,70 @@
         <v>43737</v>
       </c>
       <c r="B3" s="14">
+        <f>B2-C3</f>
         <v>18</v>
       </c>
       <c r="C3" s="12">
-        <f>B2-B3</f>
         <v>6</v>
       </c>
-      <c r="D3">
-        <v>131</v>
-      </c>
-      <c r="E3">
+      <c r="D3" s="12">
+        <v>73</v>
+      </c>
+      <c r="E3" s="12">
         <v>410</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="48">
         <f>(D3-D2)/E3*60</f>
-        <v>19.170731707317074</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+        <v>10.682926829268292</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="13">
         <v>43751</v>
       </c>
       <c r="B4" s="14">
+        <f t="shared" ref="B4:B6" si="0">B3-C4</f>
         <v>12</v>
       </c>
-      <c r="F4" s="9"/>
-    </row>
-    <row r="5" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="12">
+        <v>6</v>
+      </c>
+      <c r="D4" s="12">
+        <v>86</v>
+      </c>
+      <c r="E4" s="12">
+        <v>390</v>
+      </c>
+      <c r="F4" s="48">
+        <f>D4/E4*60</f>
+        <v>13.23076923076923</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="13">
         <v>43765</v>
       </c>
       <c r="B5" s="14">
-        <v>6</v>
-      </c>
-      <c r="F5" s="9"/>
-    </row>
-    <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+    </row>
+    <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="13">
         <v>43779</v>
       </c>
       <c r="B6" s="14">
-        <v>0</v>
-      </c>
-      <c r="F6" s="9"/>
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
@@ -45835,8 +45919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:Q1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.41015625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -45940,7 +46024,7 @@
         <v>60</v>
       </c>
       <c r="G2" s="32">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H2" s="32">
         <v>60</v>
@@ -45950,23 +46034,23 @@
       </c>
       <c r="J2" s="32"/>
       <c r="K2" s="34" t="s">
-        <v>225</v>
+        <v>246</v>
       </c>
       <c r="L2" s="34" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="M2" s="34" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="N2" s="34"/>
       <c r="O2" s="34" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="P2" s="34" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q2" s="43" t="s">
         <v>235</v>
-      </c>
-      <c r="Q2" s="43" t="s">
-        <v>241</v>
       </c>
       <c r="R2" s="32"/>
       <c r="S2" s="32"/>
@@ -45998,7 +46082,7 @@
         <v>60</v>
       </c>
       <c r="G3" s="32">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="H3" s="32">
         <v>60</v>
@@ -46008,23 +46092,23 @@
       </c>
       <c r="J3" s="32"/>
       <c r="K3" s="34" t="s">
-        <v>226</v>
+        <v>246</v>
       </c>
       <c r="L3" s="34" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="M3" s="34" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="N3" s="34"/>
       <c r="O3" s="34" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="P3" s="34" t="s">
         <v>124</v>
       </c>
       <c r="Q3" s="43" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="R3" s="32"/>
       <c r="S3" s="32"/>
@@ -46056,7 +46140,7 @@
         <v>180</v>
       </c>
       <c r="G4" s="32">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="H4" s="32">
         <v>90</v>
@@ -46066,23 +46150,23 @@
       </c>
       <c r="J4" s="32"/>
       <c r="K4" s="34" t="s">
+        <v>246</v>
+      </c>
+      <c r="L4" s="34" t="s">
         <v>218</v>
       </c>
-      <c r="L4" s="34" t="s">
-        <v>220</v>
-      </c>
       <c r="M4" s="34" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="N4" s="34"/>
       <c r="O4" s="34" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="P4" s="34" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="Q4" s="43" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="R4" s="32"/>
       <c r="S4" s="32"/>
@@ -46114,7 +46198,7 @@
         <v>180</v>
       </c>
       <c r="G5" s="32">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="H5" s="32">
         <v>120</v>
@@ -46124,23 +46208,23 @@
       </c>
       <c r="J5" s="32"/>
       <c r="K5" s="34" t="s">
+        <v>246</v>
+      </c>
+      <c r="L5" s="34" t="s">
         <v>219</v>
       </c>
-      <c r="L5" s="34" t="s">
-        <v>221</v>
-      </c>
       <c r="M5" s="34" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="N5" s="34"/>
       <c r="O5" s="34" t="s">
+        <v>220</v>
+      </c>
+      <c r="P5" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="P5" s="34" t="s">
-        <v>224</v>
-      </c>
       <c r="Q5" s="43" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="R5" s="32"/>
       <c r="S5" s="32"/>
@@ -46172,7 +46256,7 @@
         <v>60</v>
       </c>
       <c r="G6" s="32">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="H6" s="32">
         <v>20</v>
@@ -46182,23 +46266,23 @@
       </c>
       <c r="J6" s="32"/>
       <c r="K6" s="34" t="s">
-        <v>227</v>
+        <v>246</v>
       </c>
       <c r="L6" s="34" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="M6" s="34">
         <v>59</v>
       </c>
       <c r="N6" s="34"/>
       <c r="O6" s="34" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="P6" s="34" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="Q6" s="43" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="R6" s="32"/>
       <c r="S6" s="32"/>
@@ -46230,7 +46314,7 @@
         <v>60</v>
       </c>
       <c r="G7" s="32">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="H7" s="32">
         <v>60</v>
@@ -46240,23 +46324,23 @@
       </c>
       <c r="J7" s="32"/>
       <c r="K7" s="34" t="s">
-        <v>228</v>
+        <v>246</v>
       </c>
       <c r="L7" s="34" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="M7" s="34" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="N7" s="34"/>
       <c r="O7" s="34" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="P7" s="34" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="Q7" s="43" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="R7" s="32"/>
       <c r="S7" s="32"/>
@@ -46525,7 +46609,7 @@
     <row r="17" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="32"/>
       <c r="B17" s="38" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C17" s="32"/>
       <c r="D17" s="32"/>
@@ -46555,7 +46639,7 @@
     <row r="18" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="32"/>
       <c r="B18" s="38" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C18" s="32"/>
       <c r="D18" s="32"/>
@@ -46585,7 +46669,7 @@
     <row r="19" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="32"/>
       <c r="B19" s="38" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C19" s="32"/>
       <c r="D19" s="32"/>
@@ -46645,7 +46729,7 @@
     <row r="21" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="32"/>
       <c r="B21" s="38" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C21" s="32"/>
       <c r="D21" s="32"/>
@@ -46675,7 +46759,7 @@
     <row r="22" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="32"/>
       <c r="B22" s="44" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C22" s="32"/>
       <c r="D22" s="32"/>
@@ -53036,8 +53120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.41015625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -53105,14 +53189,42 @@
       <c r="C2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>13</v>
+      <c r="D2" s="4" t="s">
+        <v>217</v>
       </c>
       <c r="E2" s="12">
         <v>20</v>
       </c>
       <c r="F2" s="12">
         <v>45</v>
+      </c>
+      <c r="G2" s="35">
+        <v>16</v>
+      </c>
+      <c r="H2" s="35">
+        <v>60</v>
+      </c>
+      <c r="I2" s="45">
+        <v>43745</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="M2" s="47" t="s">
+        <v>262</v>
+      </c>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q2" s="46" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.45">
@@ -53125,14 +53237,42 @@
       <c r="C3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>13</v>
+      <c r="D3" s="4" t="s">
+        <v>217</v>
       </c>
       <c r="E3" s="12">
         <v>20</v>
       </c>
       <c r="F3" s="12">
         <v>60</v>
+      </c>
+      <c r="G3" s="35">
+        <v>14</v>
+      </c>
+      <c r="H3" s="35">
+        <v>60</v>
+      </c>
+      <c r="I3" s="45">
+        <v>43745</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="M3" s="47" t="s">
+        <v>261</v>
+      </c>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q3" s="46" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
@@ -53154,7 +53294,7 @@
       <c r="F4" s="12">
         <v>120</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="35">
         <v>11</v>
       </c>
       <c r="H4" s="6">
@@ -53163,14 +53303,24 @@
       <c r="I4" s="45">
         <v>43740</v>
       </c>
-      <c r="K4" t="s">
-        <v>252</v>
-      </c>
-      <c r="L4" t="s">
-        <v>254</v>
-      </c>
-      <c r="M4" t="s">
-        <v>256</v>
+      <c r="K4" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="M4" s="47" t="s">
+        <v>250</v>
+      </c>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q4" s="46" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
@@ -53192,7 +53342,7 @@
       <c r="F5" s="12">
         <v>120</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="35">
         <v>11</v>
       </c>
       <c r="H5" s="6">
@@ -53201,14 +53351,24 @@
       <c r="I5" s="45">
         <v>43740</v>
       </c>
-      <c r="K5" t="s">
-        <v>252</v>
-      </c>
-      <c r="L5" t="s">
-        <v>253</v>
-      </c>
-      <c r="M5" t="s">
-        <v>255</v>
+      <c r="K5" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="M5" s="47" t="s">
+        <v>249</v>
+      </c>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q5" s="46" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
@@ -53221,14 +53381,42 @@
       <c r="C6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>13</v>
+      <c r="D6" s="4" t="s">
+        <v>217</v>
       </c>
       <c r="E6" s="12">
         <v>20</v>
       </c>
       <c r="F6" s="12">
         <v>30</v>
+      </c>
+      <c r="G6" s="35">
+        <v>17</v>
+      </c>
+      <c r="H6" s="35">
+        <v>120</v>
+      </c>
+      <c r="I6" s="45">
+        <v>43744</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="M6" s="46" t="s">
+        <v>264</v>
+      </c>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q6" s="46" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
@@ -53241,14 +53429,42 @@
       <c r="C7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>13</v>
+      <c r="D7" s="4" t="s">
+        <v>217</v>
       </c>
       <c r="E7" s="12">
         <v>20</v>
       </c>
       <c r="F7" s="12">
         <v>30</v>
+      </c>
+      <c r="G7" s="35">
+        <v>17</v>
+      </c>
+      <c r="H7" s="35">
+        <v>30</v>
+      </c>
+      <c r="I7" s="45">
+        <v>43744</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="M7" s="47" t="s">
+        <v>263</v>
+      </c>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q7" s="46" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -54246,7 +54462,7 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -54254,7 +54470,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.41015625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -54302,6 +54520,15 @@
       <c r="C2" s="12" t="s">
         <v>10</v>
       </c>
+      <c r="D2" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="35">
+        <v>15</v>
+      </c>
+      <c r="F2" s="35">
+        <v>120</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="23" t="s">
@@ -54313,8 +54540,17 @@
       <c r="C3" s="12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D3" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="35">
+        <v>15</v>
+      </c>
+      <c r="F3" s="35">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>56</v>
       </c>
@@ -54324,8 +54560,17 @@
       <c r="C4" s="12" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D4" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="35">
+        <v>15</v>
+      </c>
+      <c r="F4" s="35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -54335,8 +54580,17 @@
       <c r="C5" s="12" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D5" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="35">
+        <v>15</v>
+      </c>
+      <c r="F5" s="35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>60</v>
       </c>
@@ -54346,8 +54600,17 @@
       <c r="C6" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D6" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="35">
+        <v>8</v>
+      </c>
+      <c r="F6" s="35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>62</v>
       </c>
@@ -54356,6 +54619,15 @@
       </c>
       <c r="C7" s="6" t="s">
         <v>20</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="35">
+        <v>8</v>
+      </c>
+      <c r="F7" s="35">
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -55353,7 +55625,7 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Team report - Sprint 3
</commit_message>
<xml_diff>
--- a/TeamAaronAshishJuliaReport.xlsx
+++ b/TeamAaronAshishJuliaReport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6300" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="300">
   <si>
     <t>Sprint</t>
   </si>
@@ -850,6 +850,90 @@
   <si>
     <t>Complete user stories early so there's time to discuss any issues, time to review and merge with the master branch</t>
   </si>
+  <si>
+    <t>Reviewing with TA</t>
+  </si>
+  <si>
+    <t>Trying to fix at the last minute</t>
+  </si>
+  <si>
+    <t>Updating sheets late</t>
+  </si>
+  <si>
+    <t>Waiting till the end of Sprint to complete the stories</t>
+  </si>
+  <si>
+    <t>us_09</t>
+  </si>
+  <si>
+    <t>us_11</t>
+  </si>
+  <si>
+    <t>us_30</t>
+  </si>
+  <si>
+    <t>us_31</t>
+  </si>
+  <si>
+    <t>us_23</t>
+  </si>
+  <si>
+    <t>us_24</t>
+  </si>
+  <si>
+    <t>390-419</t>
+  </si>
+  <si>
+    <t>471-500</t>
+  </si>
+  <si>
+    <t>458-468</t>
+  </si>
+  <si>
+    <t>374-383</t>
+  </si>
+  <si>
+    <t>361-371</t>
+  </si>
+  <si>
+    <t>423-455</t>
+  </si>
+  <si>
+    <t>test_us09</t>
+  </si>
+  <si>
+    <t>test_us11</t>
+  </si>
+  <si>
+    <t>test_us30</t>
+  </si>
+  <si>
+    <t>test_us31</t>
+  </si>
+  <si>
+    <t>test_us23</t>
+  </si>
+  <si>
+    <t>test_us24</t>
+  </si>
+  <si>
+    <t>121-125</t>
+  </si>
+  <si>
+    <t>130-136</t>
+  </si>
+  <si>
+    <t>140-147</t>
+  </si>
+  <si>
+    <t>151-155</t>
+  </si>
+  <si>
+    <t>159-165</t>
+  </si>
+  <si>
+    <t>169-173</t>
+  </si>
 </sst>
 </file>
 
@@ -859,7 +943,7 @@
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -967,6 +1051,19 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1007,7 +1104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1089,6 +1186,14 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1146,6 +1251,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1247,10 +1353,10 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1322,6 +1428,9 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -1462,6 +1571,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3442,7 +3552,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.41015625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -31771,7 +31883,7 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.41015625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -32278,8 +32390,8 @@
       <c r="D14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>13</v>
+      <c r="E14" s="24" t="s">
+        <v>217</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -32315,8 +32427,8 @@
       <c r="D15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>13</v>
+      <c r="E15" s="24" t="s">
+        <v>217</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -32352,8 +32464,8 @@
       <c r="D16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>13</v>
+      <c r="E16" s="24" t="s">
+        <v>217</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -32389,8 +32501,8 @@
       <c r="D17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>13</v>
+      <c r="E17" s="24" t="s">
+        <v>217</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -32426,8 +32538,8 @@
       <c r="D18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>13</v>
+      <c r="E18" s="24" t="s">
+        <v>217</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -32463,8 +32575,8 @@
       <c r="D19" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>13</v>
+      <c r="E19" s="24" t="s">
+        <v>217</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -40725,8 +40837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.41015625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -40842,12 +40954,21 @@
       </c>
       <c r="B5" s="14">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
+        <v>6</v>
+      </c>
+      <c r="C5" s="12">
+        <v>6</v>
+      </c>
+      <c r="D5" s="12">
+        <v>119</v>
+      </c>
+      <c r="E5" s="12">
+        <v>840</v>
+      </c>
+      <c r="F5" s="48">
+        <f>D5/E5*60</f>
+        <v>8.5</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="13">
@@ -40855,7 +40976,7 @@
       </c>
       <c r="B6" s="14">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
@@ -53121,8 +53242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.41015625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -54495,10 +54616,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1000"/>
+  <dimension ref="A1:Q1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.41015625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -54508,7 +54629,7 @@
     <col min="3" max="9" width="10.87890625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -54536,8 +54657,27 @@
       <c r="I1" s="17" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="K1" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="L1" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="N1" s="34"/>
+      <c r="O1" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="P1" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q1" s="33" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="23" t="s">
         <v>52</v>
       </c>
@@ -54547,8 +54687,8 @@
       <c r="C2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="23" t="s">
-        <v>13</v>
+      <c r="D2" s="52" t="s">
+        <v>217</v>
       </c>
       <c r="E2" s="35">
         <v>15</v>
@@ -54556,8 +54696,36 @@
       <c r="F2" s="35">
         <v>120</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G2">
+        <v>29</v>
+      </c>
+      <c r="H2">
+        <v>120</v>
+      </c>
+      <c r="I2" s="45">
+        <v>43763</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="L2" s="47" t="s">
+        <v>276</v>
+      </c>
+      <c r="M2" s="47" t="s">
+        <v>282</v>
+      </c>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P2" s="47" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q2" s="46" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="23" t="s">
         <v>54</v>
       </c>
@@ -54567,8 +54735,8 @@
       <c r="C3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="23" t="s">
-        <v>13</v>
+      <c r="D3" s="52" t="s">
+        <v>217</v>
       </c>
       <c r="E3" s="35">
         <v>15</v>
@@ -54576,8 +54744,36 @@
       <c r="F3" s="35">
         <v>120</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G3">
+        <v>32</v>
+      </c>
+      <c r="H3">
+        <v>180</v>
+      </c>
+      <c r="I3" s="45">
+        <v>43763</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="L3" s="47" t="s">
+        <v>277</v>
+      </c>
+      <c r="M3" s="47" t="s">
+        <v>287</v>
+      </c>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P3" s="47" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q3" s="46" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>56</v>
       </c>
@@ -54587,17 +54783,45 @@
       <c r="C4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="23" t="s">
-        <v>13</v>
+      <c r="D4" s="52" t="s">
+        <v>217</v>
       </c>
       <c r="E4" s="35">
         <v>15</v>
       </c>
       <c r="F4" s="35">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.45">
+        <v>120</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>120</v>
+      </c>
+      <c r="I4" s="45">
+        <v>43752</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="L4" s="47" t="s">
+        <v>278</v>
+      </c>
+      <c r="M4" s="47" t="s">
+        <v>286</v>
+      </c>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P4" s="47" t="s">
+        <v>290</v>
+      </c>
+      <c r="Q4" s="46" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -54607,17 +54831,45 @@
       <c r="C5" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="23" t="s">
-        <v>13</v>
+      <c r="D5" s="52" t="s">
+        <v>217</v>
       </c>
       <c r="E5" s="35">
         <v>15</v>
       </c>
       <c r="F5" s="35">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.45">
+        <v>120</v>
+      </c>
+      <c r="G5">
+        <v>9</v>
+      </c>
+      <c r="H5">
+        <v>120</v>
+      </c>
+      <c r="I5" s="45">
+        <v>43752</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="L5" s="47" t="s">
+        <v>279</v>
+      </c>
+      <c r="M5" s="47" t="s">
+        <v>285</v>
+      </c>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P5" s="47" t="s">
+        <v>291</v>
+      </c>
+      <c r="Q5" s="46" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>60</v>
       </c>
@@ -54627,8 +54879,8 @@
       <c r="C6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>13</v>
+      <c r="D6" s="52" t="s">
+        <v>217</v>
       </c>
       <c r="E6" s="35">
         <v>8</v>
@@ -54636,8 +54888,36 @@
       <c r="F6" s="35">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6" s="35">
+        <v>120</v>
+      </c>
+      <c r="I6" s="45">
+        <v>43765</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="L6" s="47" t="s">
+        <v>280</v>
+      </c>
+      <c r="M6" s="46" t="s">
+        <v>284</v>
+      </c>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P6" s="47" t="s">
+        <v>292</v>
+      </c>
+      <c r="Q6" s="46" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>62</v>
       </c>
@@ -54647,8 +54927,8 @@
       <c r="C7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="23" t="s">
-        <v>13</v>
+      <c r="D7" s="52" t="s">
+        <v>217</v>
       </c>
       <c r="E7" s="35">
         <v>8</v>
@@ -54656,32 +54936,90 @@
       <c r="F7" s="35">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="17" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="18" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="19" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="G7">
+        <v>29</v>
+      </c>
+      <c r="H7">
+        <v>180</v>
+      </c>
+      <c r="I7" s="45">
+        <v>43765</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="L7" s="47" t="s">
+        <v>281</v>
+      </c>
+      <c r="M7" s="47" t="s">
+        <v>283</v>
+      </c>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="P7" s="47" t="s">
+        <v>293</v>
+      </c>
+      <c r="Q7" s="46" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="50" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="49" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="49" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="49"/>
+    </row>
+    <row r="16" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="50" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="49" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="49" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="51" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="34" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="35" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -55660,7 +55998,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.41015625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -55708,6 +56048,15 @@
       <c r="C2" s="22" t="s">
         <v>10</v>
       </c>
+      <c r="D2" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="52">
+        <v>15</v>
+      </c>
+      <c r="F2" s="52">
+        <v>120</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="23" t="s">
@@ -55719,8 +56068,17 @@
       <c r="C3" s="22" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D3" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="52">
+        <v>8</v>
+      </c>
+      <c r="F3" s="52">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>74</v>
       </c>
@@ -55730,8 +56088,17 @@
       <c r="C4" s="12" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D4" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="52">
+        <v>10</v>
+      </c>
+      <c r="F4" s="52">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
         <v>82</v>
       </c>
@@ -55741,8 +56108,17 @@
       <c r="C5" s="12" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D5" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="52">
+        <v>15</v>
+      </c>
+      <c r="F5" s="52">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>85</v>
       </c>
@@ -55752,8 +56128,17 @@
       <c r="C6" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D6" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="52">
+        <v>25</v>
+      </c>
+      <c r="F6" s="52">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>87</v>
       </c>
@@ -55762,6 +56147,15 @@
       </c>
       <c r="C7" s="6" t="s">
         <v>20</v>
+      </c>
+      <c r="D7" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="52">
+        <v>25</v>
+      </c>
+      <c r="F7" s="52">
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Team report - Sprint 4
</commit_message>
<xml_diff>
--- a/TeamAaronAshishJuliaReport.xlsx
+++ b/TeamAaronAshishJuliaReport.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="329">
   <si>
     <t>Sprint</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Marriage before divorce</t>
-  </si>
-  <si>
-    <t>Incomplete</t>
   </si>
   <si>
     <t>Julia</t>
@@ -934,6 +931,96 @@
   <si>
     <t>169-173</t>
   </si>
+  <si>
+    <t>11/6/2019</t>
+  </si>
+  <si>
+    <t>test_us15</t>
+  </si>
+  <si>
+    <t>test_us21</t>
+  </si>
+  <si>
+    <t>test_us29</t>
+  </si>
+  <si>
+    <t>test_us34</t>
+  </si>
+  <si>
+    <t>test_us18</t>
+  </si>
+  <si>
+    <t>test_us17</t>
+  </si>
+  <si>
+    <t>us_15</t>
+  </si>
+  <si>
+    <t>us_21</t>
+  </si>
+  <si>
+    <t>us_29</t>
+  </si>
+  <si>
+    <t>us_34</t>
+  </si>
+  <si>
+    <t>us_18</t>
+  </si>
+  <si>
+    <t>us_17</t>
+  </si>
+  <si>
+    <t>11/4/2019</t>
+  </si>
+  <si>
+    <t>10/31/2019</t>
+  </si>
+  <si>
+    <t>566-590</t>
+  </si>
+  <si>
+    <t>593-637</t>
+  </si>
+  <si>
+    <t>542-547</t>
+  </si>
+  <si>
+    <t>550-563</t>
+  </si>
+  <si>
+    <t>512-520</t>
+  </si>
+  <si>
+    <t>523-539</t>
+  </si>
+  <si>
+    <t>Complete stories early, like in Sprint-4 to avoid last minute stress</t>
+  </si>
+  <si>
+    <t>Highlight issues early</t>
+  </si>
+  <si>
+    <t>Not updating the IDs in test files to prevent clash with IDs in other user stories</t>
+  </si>
+  <si>
+    <t>192-196</t>
+  </si>
+  <si>
+    <t>199-203</t>
+  </si>
+  <si>
+    <t>176-182</t>
+  </si>
+  <si>
+    <t>185-189</t>
+  </si>
+  <si>
+    <t>207-211</t>
+  </si>
+  <si>
+    <t>215-219</t>
+  </si>
 </sst>
 </file>
 
@@ -1104,7 +1191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1194,6 +1281,11 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1356,7 +1448,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1431,6 +1523,9 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -2487,52 +2582,52 @@
         <v>10</v>
       </c>
       <c r="B3" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="D3" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="41" t="s">
-        <v>16</v>
-      </c>
       <c r="E3" s="32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3" s="32"/>
       <c r="G3" s="32"/>
     </row>
     <row r="4" spans="1:25" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="C4" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="D4" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="41" t="s">
-        <v>23</v>
-      </c>
       <c r="E4" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="C5" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="D5" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="E5" s="32" t="s">
         <v>30</v>
-      </c>
-      <c r="E5" s="32" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="12" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -2540,10 +2635,10 @@
     <row r="8" spans="1:25" ht="12" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="9" spans="1:25" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D9" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="42" t="s">
         <v>32</v>
-      </c>
-      <c r="E9" s="42" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="12" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -3553,7 +3648,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.41015625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3572,7 +3667,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>4</v>
@@ -3602,16 +3697,16 @@
     </row>
     <row r="2" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="C2" s="25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="24"/>
       <c r="F2" s="24"/>
@@ -3638,13 +3733,13 @@
     </row>
     <row r="3" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="25" t="s">
         <v>143</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>144</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="24"/>
@@ -3672,13 +3767,13 @@
     </row>
     <row r="4" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>105</v>
-      </c>
       <c r="C4" s="25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="24"/>
@@ -3712,7 +3807,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>10</v>
@@ -3742,13 +3837,13 @@
     </row>
     <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="C6" s="25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>10</v>
@@ -3778,13 +3873,13 @@
     </row>
     <row r="7" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="C7" s="25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>10</v>
@@ -3814,13 +3909,13 @@
     </row>
     <row r="8" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="C8" s="25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>10</v>
@@ -3850,16 +3945,16 @@
     </row>
     <row r="9" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="C9" s="25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9" s="24"/>
       <c r="F9" s="24"/>
@@ -3886,13 +3981,13 @@
     </row>
     <row r="10" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="C10" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>10</v>
@@ -3922,13 +4017,13 @@
     </row>
     <row r="11" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="25" t="s">
         <v>153</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>154</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="24"/>
@@ -3956,13 +4051,13 @@
     </row>
     <row r="12" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="C12" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>10</v>
@@ -3992,13 +4087,13 @@
     </row>
     <row r="13" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="C13" s="25" t="s">
         <v>157</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>158</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="24"/>
@@ -4026,13 +4121,13 @@
     </row>
     <row r="14" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="C14" s="25" t="s">
         <v>160</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>161</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="24"/>
@@ -4060,13 +4155,13 @@
     </row>
     <row r="15" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="C15" s="25" t="s">
         <v>163</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>164</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="24"/>
@@ -4094,13 +4189,13 @@
     </row>
     <row r="16" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>66</v>
-      </c>
       <c r="C16" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>10</v>
@@ -4130,16 +4225,16 @@
     </row>
     <row r="17" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="C17" s="25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17" s="24"/>
       <c r="F17" s="24"/>
@@ -4166,16 +4261,16 @@
     </row>
     <row r="18" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>88</v>
-      </c>
       <c r="C18" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E18" s="24"/>
       <c r="F18" s="24"/>
@@ -4202,16 +4297,16 @@
     </row>
     <row r="19" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>86</v>
-      </c>
       <c r="C19" s="25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E19" s="24"/>
       <c r="F19" s="24"/>
@@ -4238,13 +4333,13 @@
     </row>
     <row r="20" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="C20" s="25" t="s">
         <v>170</v>
-      </c>
-      <c r="C20" s="25" t="s">
-        <v>171</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="24"/>
@@ -4272,13 +4367,13 @@
     </row>
     <row r="21" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="C21" s="25" t="s">
         <v>173</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>174</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="24"/>
@@ -4306,13 +4401,13 @@
     </row>
     <row r="22" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>69</v>
-      </c>
       <c r="C22" s="25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>10</v>
@@ -4342,16 +4437,16 @@
     </row>
     <row r="23" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="C23" s="25" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E23" s="24"/>
       <c r="F23" s="24"/>
@@ -4378,16 +4473,16 @@
     </row>
     <row r="24" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="C24" s="25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E24" s="24"/>
       <c r="F24" s="24"/>
@@ -4414,16 +4509,16 @@
     </row>
     <row r="25" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>63</v>
-      </c>
       <c r="C25" s="25" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E25" s="24"/>
       <c r="F25" s="24"/>
@@ -4450,13 +4545,13 @@
     </row>
     <row r="26" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="C26" s="25" t="s">
         <v>180</v>
-      </c>
-      <c r="C26" s="25" t="s">
-        <v>181</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="24"/>
@@ -4484,13 +4579,13 @@
     </row>
     <row r="27" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="C27" s="25" t="s">
         <v>183</v>
-      </c>
-      <c r="C27" s="25" t="s">
-        <v>184</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="24"/>
@@ -4518,13 +4613,13 @@
     </row>
     <row r="28" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="C28" s="25" t="s">
         <v>186</v>
-      </c>
-      <c r="C28" s="25" t="s">
-        <v>187</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="24"/>
@@ -4552,13 +4647,13 @@
     </row>
     <row r="29" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="C29" s="25" t="s">
         <v>189</v>
-      </c>
-      <c r="C29" s="25" t="s">
-        <v>190</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="24"/>
@@ -4586,16 +4681,16 @@
     </row>
     <row r="30" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="B30" s="26" t="s">
-        <v>75</v>
-      </c>
       <c r="C30" s="27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E30" s="24"/>
       <c r="F30" s="24"/>
@@ -4622,16 +4717,16 @@
     </row>
     <row r="31" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="26" t="s">
-        <v>57</v>
-      </c>
       <c r="C31" s="27" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
@@ -4658,16 +4753,16 @@
     </row>
     <row r="32" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="B32" s="26" t="s">
-        <v>59</v>
-      </c>
       <c r="C32" s="27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E32" s="24"/>
       <c r="F32" s="24"/>
@@ -4694,13 +4789,13 @@
     </row>
     <row r="33" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="C33" s="25" t="s">
         <v>195</v>
-      </c>
-      <c r="C33" s="25" t="s">
-        <v>196</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="24"/>
@@ -4728,13 +4823,13 @@
     </row>
     <row r="34" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="C34" s="25" t="s">
         <v>198</v>
-      </c>
-      <c r="C34" s="25" t="s">
-        <v>199</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="24"/>
@@ -4762,16 +4857,16 @@
     </row>
     <row r="35" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="B35" s="26" t="s">
-        <v>83</v>
-      </c>
       <c r="C35" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E35" s="24"/>
       <c r="F35" s="24"/>
@@ -4798,16 +4893,16 @@
     </row>
     <row r="36" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B36" s="26" t="s">
-        <v>47</v>
-      </c>
       <c r="C36" s="27" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E36" s="24"/>
       <c r="F36" s="24"/>
@@ -4834,16 +4929,16 @@
     </row>
     <row r="37" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A37" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="26" t="s">
-        <v>45</v>
-      </c>
       <c r="C37" s="27" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E37" s="24"/>
       <c r="F37" s="24"/>
@@ -4870,13 +4965,13 @@
     </row>
     <row r="38" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A38" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="C38" s="25" t="s">
         <v>204</v>
-      </c>
-      <c r="C38" s="25" t="s">
-        <v>205</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="24"/>
@@ -4904,16 +4999,16 @@
     </row>
     <row r="39" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A39" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="26" t="s">
-        <v>35</v>
-      </c>
       <c r="C39" s="27" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E39" s="24"/>
       <c r="F39" s="24"/>
@@ -4940,13 +5035,13 @@
     </row>
     <row r="40" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A40" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="C40" s="25" t="s">
         <v>208</v>
-      </c>
-      <c r="C40" s="25" t="s">
-        <v>209</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="24"/>
@@ -4974,13 +5069,13 @@
     </row>
     <row r="41" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A41" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="C41" s="25" t="s">
         <v>211</v>
-      </c>
-      <c r="C41" s="25" t="s">
-        <v>212</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="24"/>
@@ -5008,13 +5103,13 @@
     </row>
     <row r="42" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A42" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="C42" s="25" t="s">
         <v>214</v>
-      </c>
-      <c r="C42" s="25" t="s">
-        <v>215</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="24"/>
@@ -5042,16 +5137,16 @@
     </row>
     <row r="43" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A43" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="26" t="s">
-        <v>25</v>
-      </c>
       <c r="C43" s="27" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E43" s="24"/>
       <c r="F43" s="24"/>
@@ -31883,7 +31978,7 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.41015625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -31947,7 +32042,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -31975,16 +32070,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -32012,16 +32107,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -32049,16 +32144,16 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -32086,16 +32181,16 @@
         <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
@@ -32123,16 +32218,16 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -32160,16 +32255,16 @@
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -32197,16 +32292,16 @@
         <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -32234,16 +32329,16 @@
         <v>2</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -32271,16 +32366,16 @@
         <v>2</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -32308,16 +32403,16 @@
         <v>2</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="D12" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -32345,16 +32440,16 @@
         <v>2</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="D13" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -32382,16 +32477,16 @@
         <v>3</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>52</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>53</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -32419,16 +32514,16 @@
         <v>3</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>55</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -32456,16 +32551,16 @@
         <v>3</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="D16" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -32493,16 +32588,16 @@
         <v>3</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -32530,16 +32625,16 @@
         <v>3</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="D18" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -32567,16 +32662,16 @@
         <v>3</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>63</v>
-      </c>
       <c r="D19" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -32604,16 +32699,16 @@
         <v>4</v>
       </c>
       <c r="B20" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>66</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>13</v>
+      <c r="E20" s="24" t="s">
+        <v>216</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -32641,16 +32736,16 @@
         <v>4</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>69</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>13</v>
+      <c r="E21" s="24" t="s">
+        <v>216</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -32678,16 +32773,16 @@
         <v>4</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="D22" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>13</v>
+        <v>26</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>216</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -32715,16 +32810,16 @@
         <v>4</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="D23" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>13</v>
+        <v>26</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>216</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -32752,16 +32847,16 @@
         <v>4</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>86</v>
-      </c>
       <c r="D24" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>13</v>
+        <v>19</v>
+      </c>
+      <c r="E24" s="24" t="s">
+        <v>216</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
@@ -32789,16 +32884,16 @@
         <v>4</v>
       </c>
       <c r="B25" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>88</v>
-      </c>
       <c r="D25" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>13</v>
+        <v>19</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>216</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
@@ -39006,7 +39101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -39023,19 +39118,19 @@
   <sheetData>
     <row r="1" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F3" s="9"/>
     </row>
@@ -39045,13 +39140,13 @@
     </row>
     <row r="5" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F6" s="9"/>
     </row>
@@ -39061,7 +39156,7 @@
     </row>
     <row r="8" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F8" s="9"/>
     </row>
@@ -39090,22 +39185,22 @@
         <v>0</v>
       </c>
       <c r="B14" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="11" t="s">
         <v>80</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>81</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -39129,7 +39224,7 @@
     </row>
     <row r="15" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B15" s="13">
         <v>43723</v>
@@ -39145,7 +39240,7 @@
     </row>
     <row r="16" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B16" s="13">
         <v>43737</v>
@@ -39170,7 +39265,7 @@
     </row>
     <row r="17" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B17" s="13">
         <v>43751</v>
@@ -39195,7 +39290,7 @@
     </row>
     <row r="18" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B18" s="13">
         <v>43765</v>
@@ -39220,7 +39315,7 @@
     </row>
     <row r="19" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B19" s="13">
         <v>43779</v>
@@ -40837,8 +40932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.41015625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -40854,22 +40949,22 @@
   <sheetData>
     <row r="1" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="11" t="s">
         <v>80</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>81</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -40976,12 +41071,21 @@
       </c>
       <c r="B6" s="14">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C6" s="12">
         <v>6</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
+      <c r="D6" s="12">
+        <v>116</v>
+      </c>
+      <c r="E6" s="12">
+        <v>780</v>
+      </c>
+      <c r="F6" s="48">
+        <f>D6/E6*60</f>
+        <v>8.9230769230769234</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
@@ -42669,52 +42773,52 @@
         <v>5</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="G1" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="H1" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="I1" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="K1" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="L1" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="M1" s="19" t="s">
         <v>99</v>
-      </c>
-      <c r="M1" s="19" t="s">
-        <v>100</v>
       </c>
       <c r="N1" s="20"/>
       <c r="O1" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="P1" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="P1" s="19" t="s">
+      <c r="Q1" s="19" t="s">
         <v>102</v>
-      </c>
-      <c r="Q1" s="19" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="C2" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>106</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>107</v>
       </c>
       <c r="E2" s="12">
         <v>150</v>
@@ -42732,23 +42836,23 @@
         <v>41906</v>
       </c>
       <c r="K2" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="L2" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="M2" s="20" t="s">
         <v>109</v>
-      </c>
-      <c r="M2" s="20" t="s">
-        <v>110</v>
       </c>
       <c r="N2" s="20"/>
       <c r="O2" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="P2" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="P2" s="20" t="s">
+      <c r="Q2" s="20" t="s">
         <v>112</v>
-      </c>
-      <c r="Q2" s="20" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -42764,13 +42868,13 @@
     </row>
     <row r="4" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="B4" s="21" t="s">
-        <v>115</v>
-      </c>
       <c r="C4" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I4" s="8"/>
       <c r="K4" s="20"/>
@@ -42783,13 +42887,13 @@
     </row>
     <row r="5" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="B5" s="21" t="s">
-        <v>117</v>
-      </c>
       <c r="C5" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I5" s="8"/>
       <c r="K5" s="20"/>
@@ -42802,13 +42906,13 @@
     </row>
     <row r="6" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="B6" s="21" t="s">
-        <v>119</v>
-      </c>
       <c r="C6" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I6" s="8"/>
       <c r="K6" s="20"/>
@@ -42832,16 +42936,16 @@
     </row>
     <row r="8" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="21" t="s">
-        <v>18</v>
-      </c>
       <c r="C8" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>120</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>121</v>
       </c>
       <c r="E8" s="12">
         <v>200</v>
@@ -42851,23 +42955,23 @@
       </c>
       <c r="I8" s="8"/>
       <c r="K8" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L8" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M8" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N8" s="20"/>
       <c r="O8" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="P8" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="P8" s="20" t="s">
+      <c r="Q8" s="20" t="s">
         <v>124</v>
-      </c>
-      <c r="Q8" s="20" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -42883,16 +42987,16 @@
     </row>
     <row r="10" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="C10" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>128</v>
-      </c>
       <c r="D10" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I10" s="8"/>
       <c r="K10" s="20"/>
@@ -42905,13 +43009,13 @@
     </row>
     <row r="11" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B11" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="B11" s="21" t="s">
-        <v>130</v>
-      </c>
       <c r="C11" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I11" s="8"/>
       <c r="K11" s="20"/>
@@ -42924,13 +43028,13 @@
     </row>
     <row r="12" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="C12" s="12" t="s">
         <v>132</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>133</v>
       </c>
       <c r="I12" s="8"/>
       <c r="K12" s="20"/>
@@ -42954,7 +43058,7 @@
     </row>
     <row r="14" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I14" s="8"/>
       <c r="K14" s="20"/>
@@ -42978,7 +43082,7 @@
     </row>
     <row r="16" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I16" s="8"/>
       <c r="K16" s="20"/>
@@ -42991,7 +43095,7 @@
     </row>
     <row r="17" spans="2:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I17" s="8"/>
       <c r="K17" s="20"/>
@@ -43004,7 +43108,7 @@
     </row>
     <row r="18" spans="2:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I18" s="8"/>
       <c r="K18" s="20"/>
@@ -43028,7 +43132,7 @@
     </row>
     <row r="20" spans="2:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I20" s="8"/>
       <c r="K20" s="20"/>
@@ -43041,7 +43145,7 @@
     </row>
     <row r="21" spans="2:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I21" s="8"/>
       <c r="K21" s="20"/>
@@ -46042,7 +46146,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:B22"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.41015625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -46082,39 +46186,39 @@
         <v>5</v>
       </c>
       <c r="E1" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="G1" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="H1" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="I1" s="31" t="s">
         <v>96</v>
-      </c>
-      <c r="I1" s="31" t="s">
-        <v>97</v>
       </c>
       <c r="J1" s="32"/>
       <c r="K1" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="M1" s="33" t="s">
         <v>99</v>
-      </c>
-      <c r="M1" s="33" t="s">
-        <v>100</v>
       </c>
       <c r="N1" s="34"/>
       <c r="O1" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="P1" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="P1" s="33" t="s">
+      <c r="Q1" s="33" t="s">
         <v>102</v>
-      </c>
-      <c r="Q1" s="33" t="s">
-        <v>103</v>
       </c>
       <c r="R1" s="32"/>
       <c r="S1" s="32"/>
@@ -46137,7 +46241,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E2" s="32">
         <v>8</v>
@@ -46156,23 +46260,23 @@
       </c>
       <c r="J2" s="32"/>
       <c r="K2" s="34" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L2" s="34" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M2" s="34" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N2" s="34"/>
       <c r="O2" s="34" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P2" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="Q2" s="43" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="R2" s="32"/>
       <c r="S2" s="32"/>
@@ -46186,16 +46290,16 @@
     </row>
     <row r="3" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="36" t="s">
         <v>17</v>
-      </c>
-      <c r="B3" s="36" t="s">
-        <v>18</v>
       </c>
       <c r="C3" s="36" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E3" s="32">
         <v>8</v>
@@ -46214,23 +46318,23 @@
       </c>
       <c r="J3" s="32"/>
       <c r="K3" s="34" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L3" s="34" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="M3" s="34" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N3" s="34"/>
       <c r="O3" s="34" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P3" s="34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q3" s="43" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="R3" s="32"/>
       <c r="S3" s="32"/>
@@ -46244,16 +46348,16 @@
     </row>
     <row r="4" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="38" t="s">
-        <v>25</v>
-      </c>
       <c r="C4" s="36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E4" s="36">
         <v>30</v>
@@ -46272,23 +46376,23 @@
       </c>
       <c r="J4" s="32"/>
       <c r="K4" s="34" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L4" s="34" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="M4" s="34" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N4" s="34"/>
       <c r="O4" s="34" t="s">
+        <v>219</v>
+      </c>
+      <c r="P4" s="34" t="s">
         <v>220</v>
       </c>
-      <c r="P4" s="34" t="s">
-        <v>221</v>
-      </c>
       <c r="Q4" s="43" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="R4" s="32"/>
       <c r="S4" s="32"/>
@@ -46302,16 +46406,16 @@
     </row>
     <row r="5" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="38" t="s">
-        <v>35</v>
-      </c>
       <c r="C5" s="36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E5" s="36">
         <v>30</v>
@@ -46330,23 +46434,23 @@
       </c>
       <c r="J5" s="32"/>
       <c r="K5" s="34" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L5" s="34" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M5" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="N5" s="34"/>
       <c r="O5" s="34" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P5" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Q5" s="43" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="R5" s="32"/>
       <c r="S5" s="32"/>
@@ -46360,16 +46464,16 @@
     </row>
     <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="36" t="s">
-        <v>37</v>
-      </c>
       <c r="C6" s="36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E6" s="35">
         <v>8</v>
@@ -46388,23 +46492,23 @@
       </c>
       <c r="J6" s="32"/>
       <c r="K6" s="34" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L6" s="34" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="M6" s="34">
         <v>59</v>
       </c>
       <c r="N6" s="34"/>
       <c r="O6" s="34" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P6" s="34" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="Q6" s="43" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="R6" s="32"/>
       <c r="S6" s="32"/>
@@ -46418,16 +46522,16 @@
     </row>
     <row r="7" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="36" t="s">
-        <v>39</v>
-      </c>
       <c r="C7" s="36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E7" s="35">
         <v>20</v>
@@ -46446,23 +46550,23 @@
       </c>
       <c r="J7" s="32"/>
       <c r="K7" s="34" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L7" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M7" s="34" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N7" s="34"/>
       <c r="O7" s="34" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P7" s="34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="Q7" s="43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="R7" s="32"/>
       <c r="S7" s="32"/>
@@ -46701,7 +46805,7 @@
     <row r="16" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="32"/>
       <c r="B16" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C16" s="32"/>
       <c r="D16" s="32"/>
@@ -46731,7 +46835,7 @@
     <row r="17" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="32"/>
       <c r="B17" s="38" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C17" s="32"/>
       <c r="D17" s="32"/>
@@ -46761,7 +46865,7 @@
     <row r="18" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="32"/>
       <c r="B18" s="38" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C18" s="32"/>
       <c r="D18" s="32"/>
@@ -46791,7 +46895,7 @@
     <row r="19" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="32"/>
       <c r="B19" s="38" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C19" s="32"/>
       <c r="D19" s="32"/>
@@ -46821,7 +46925,7 @@
     <row r="20" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="32"/>
       <c r="B20" s="29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C20" s="32"/>
       <c r="D20" s="32"/>
@@ -46851,7 +46955,7 @@
     <row r="21" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="32"/>
       <c r="B21" s="38" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C21" s="32"/>
       <c r="D21" s="32"/>
@@ -46881,7 +46985,7 @@
     <row r="22" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="32"/>
       <c r="B22" s="44" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C22" s="32"/>
       <c r="D22" s="32"/>
@@ -53267,52 +53371,52 @@
         <v>5</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="G1" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="H1" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="I1" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="K1" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="L1" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="M1" s="33" t="s">
         <v>99</v>
-      </c>
-      <c r="M1" s="33" t="s">
-        <v>100</v>
       </c>
       <c r="N1" s="34"/>
       <c r="O1" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="P1" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="P1" s="33" t="s">
+      <c r="Q1" s="33" t="s">
         <v>102</v>
-      </c>
-      <c r="Q1" s="33" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>40</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>41</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E2" s="12">
         <v>20</v>
@@ -53330,37 +53434,37 @@
         <v>43745</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="M2" s="47" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="N2" s="4"/>
       <c r="O2" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q2" s="46" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>42</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>43</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E3" s="12">
         <v>20</v>
@@ -53378,37 +53482,37 @@
         <v>43745</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="M3" s="47" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="N3" s="4"/>
       <c r="O3" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="Q3" s="46" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>45</v>
-      </c>
       <c r="C4" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E4" s="12">
         <v>30</v>
@@ -53426,37 +53530,37 @@
         <v>43740</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="M4" s="47" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Q4" s="46" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>47</v>
-      </c>
       <c r="C5" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E5" s="12">
         <v>30</v>
@@ -53474,37 +53578,37 @@
         <v>43740</v>
       </c>
       <c r="K5" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="L5" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="L5" s="4" t="s">
-        <v>247</v>
-      </c>
       <c r="M5" s="47" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Q5" s="46" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="C6" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E6" s="12">
         <v>20</v>
@@ -53522,37 +53626,37 @@
         <v>43744</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M6" s="46" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Q6" s="46" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="C7" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E7" s="12">
         <v>20</v>
@@ -53570,23 +53674,23 @@
         <v>43744</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="M7" s="47" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="N7" s="4"/>
       <c r="O7" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="Q7" s="46" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -53594,32 +53698,32 @@
     <row r="10" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="G11" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="G12" s="44" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="G13" s="44" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="G14" s="44" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="G15" s="29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="G16" s="44" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="17" spans="7:7" ht="12" customHeight="1" x14ac:dyDescent="0.4">
@@ -54619,7 +54723,7 @@
   <dimension ref="A1:Q1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="B12" sqref="B12:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.41015625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -54643,52 +54747,52 @@
         <v>5</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="G1" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="H1" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="I1" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="K1" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="L1" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="M1" s="33" t="s">
         <v>99</v>
-      </c>
-      <c r="M1" s="33" t="s">
-        <v>100</v>
       </c>
       <c r="N1" s="34"/>
       <c r="O1" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="P1" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="P1" s="33" t="s">
+      <c r="Q1" s="33" t="s">
         <v>102</v>
-      </c>
-      <c r="Q1" s="33" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="23" t="s">
         <v>52</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>53</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="52" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E2" s="35">
         <v>15</v>
@@ -54706,37 +54810,37 @@
         <v>43763</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L2" s="47" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="M2" s="47" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="N2" s="4"/>
       <c r="O2" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P2" s="47" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="Q2" s="46" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="23" t="s">
         <v>54</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>55</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="52" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E3" s="35">
         <v>15</v>
@@ -54754,37 +54858,37 @@
         <v>43763</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L3" s="47" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="M3" s="47" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="N3" s="4"/>
       <c r="O3" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P3" s="47" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="Q3" s="46" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>57</v>
-      </c>
       <c r="C4" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E4" s="35">
         <v>15</v>
@@ -54802,37 +54906,37 @@
         <v>43752</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L4" s="47" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="M4" s="47" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P4" s="47" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="Q4" s="46" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>59</v>
-      </c>
       <c r="C5" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E5" s="35">
         <v>15</v>
@@ -54850,37 +54954,37 @@
         <v>43752</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L5" s="47" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="M5" s="47" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P5" s="47" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="Q5" s="46" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="C6" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E6" s="35">
         <v>8</v>
@@ -54898,37 +55002,37 @@
         <v>43765</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L6" s="47" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="M6" s="46" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P6" s="47" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="Q6" s="46" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>63</v>
-      </c>
       <c r="C7" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E7" s="35">
         <v>8</v>
@@ -54946,23 +55050,23 @@
         <v>43765</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L7" s="47" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="M7" s="47" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="N7" s="4"/>
       <c r="O7" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P7" s="47" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="Q7" s="46" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -54971,17 +55075,17 @@
     <row r="11" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="50" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="49" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" s="49" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
@@ -54989,22 +55093,22 @@
     </row>
     <row r="16" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B16" s="50" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="49" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B18" s="49" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="51" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -55996,10 +56100,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1000"/>
+  <dimension ref="A1:O1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.41015625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -56009,7 +56113,7 @@
     <col min="3" max="9" width="10.87890625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -56023,33 +56127,51 @@
         <v>5</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="G1" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="H1" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="I1" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="J1" s="33" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="K1" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="L1" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="N1" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="O1" s="33" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="23" t="s">
         <v>65</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>66</v>
       </c>
       <c r="C2" s="22" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="52" t="s">
-        <v>13</v>
+        <v>216</v>
       </c>
       <c r="E2" s="52">
         <v>15</v>
@@ -56057,19 +56179,46 @@
       <c r="F2" s="52">
         <v>120</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G2" s="4">
+        <v>6</v>
+      </c>
+      <c r="H2" s="4">
+        <v>120</v>
+      </c>
+      <c r="I2" s="53" t="s">
+        <v>312</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="N2" s="47" t="s">
+        <v>300</v>
+      </c>
+      <c r="O2" s="46" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="23" t="s">
         <v>68</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>69</v>
       </c>
       <c r="C3" s="22" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="52" t="s">
-        <v>13</v>
+        <v>216</v>
       </c>
       <c r="E3" s="52">
         <v>8</v>
@@ -56077,19 +56226,46 @@
       <c r="F3" s="52">
         <v>90</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G3" s="4">
+        <v>14</v>
+      </c>
+      <c r="H3" s="4">
+        <v>120</v>
+      </c>
+      <c r="I3" s="53" t="s">
+        <v>312</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="N3" s="47" t="s">
+        <v>301</v>
+      </c>
+      <c r="O3" s="46" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>75</v>
-      </c>
       <c r="C4" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>13</v>
+        <v>216</v>
       </c>
       <c r="E4" s="52">
         <v>10</v>
@@ -56097,19 +56273,46 @@
       <c r="F4" s="52">
         <v>90</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G4" s="4">
+        <v>9</v>
+      </c>
+      <c r="H4" s="4">
+        <v>60</v>
+      </c>
+      <c r="I4" s="53" t="s">
+        <v>313</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="N4" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="O4" s="46" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>83</v>
-      </c>
       <c r="C5" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>13</v>
+        <v>216</v>
       </c>
       <c r="E5" s="52">
         <v>15</v>
@@ -56117,19 +56320,46 @@
       <c r="F5" s="52">
         <v>90</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G5" s="4">
+        <v>17</v>
+      </c>
+      <c r="H5" s="4">
+        <v>60</v>
+      </c>
+      <c r="I5" s="53" t="s">
+        <v>313</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="N5" s="47" t="s">
+        <v>303</v>
+      </c>
+      <c r="O5" s="46" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>86</v>
-      </c>
       <c r="C6" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>13</v>
+        <v>216</v>
       </c>
       <c r="E6" s="52">
         <v>25</v>
@@ -56137,19 +56367,46 @@
       <c r="F6" s="52">
         <v>120</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G6" s="4">
+        <v>45</v>
+      </c>
+      <c r="H6" s="4">
+        <v>240</v>
+      </c>
+      <c r="I6" s="53" t="s">
+        <v>299</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="N6" s="47" t="s">
+        <v>304</v>
+      </c>
+      <c r="O6" s="46" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>88</v>
-      </c>
       <c r="C7" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>13</v>
+        <v>216</v>
       </c>
       <c r="E7" s="52">
         <v>25</v>
@@ -56157,32 +56414,89 @@
       <c r="F7" s="52">
         <v>120</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="17" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="18" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="19" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="G7" s="4">
+        <v>25</v>
+      </c>
+      <c r="H7" s="4">
+        <v>180</v>
+      </c>
+      <c r="I7" s="53" t="s">
+        <v>299</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="N7" s="47" t="s">
+        <v>305</v>
+      </c>
+      <c r="O7" s="46" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C12" s="54" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C13" s="55" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C14" s="55" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C15" s="55" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C16" s="51" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C17" s="51"/>
+    </row>
+    <row r="18" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C18" s="54" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C19" s="55" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="3:3" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="34" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="35" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>